<commit_message>
Added Refunds To Spreadsheet
</commit_message>
<xml_diff>
--- a/NeatoScan/Dashboard_Site/Daily_report_Spreadsheet/Daily _Report.xlsx
+++ b/NeatoScan/Dashboard_Site/Daily_report_Spreadsheet/Daily _Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="108">
   <si>
     <t>STORE PERFORMANCE OVERVIEW</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Daily Sales</t>
   </si>
   <si>
-    <t>$5908.56</t>
+    <t>$4633.68</t>
   </si>
   <si>
     <t>Budget</t>
@@ -209,7 +209,10 @@
     <t>Sell Thru Rate</t>
   </si>
   <si>
-    <t/>
+    <t>CALC</t>
+  </si>
+  <si>
+    <t>Daily Sales Other</t>
   </si>
   <si>
     <t>Actual Sales</t>
@@ -242,6 +245,9 @@
     <t>MTD Budget Variance</t>
   </si>
   <si>
+    <t>Calc</t>
+  </si>
+  <si>
     <t>Daily Variance (%)</t>
   </si>
   <si>
@@ -333,24 +339,6 @@
   </si>
   <si>
     <t>Active eBay Listings</t>
-  </si>
-  <si>
-    <t>LABOR</t>
-  </si>
-  <si>
-    <t>Budgeted Labor</t>
-  </si>
-  <si>
-    <t>Budgeted Labor Daily</t>
-  </si>
-  <si>
-    <t>Actual Labor</t>
-  </si>
-  <si>
-    <t>Variance $</t>
-  </si>
-  <si>
-    <t>Labor Hours</t>
   </si>
 </sst>
 </file>
@@ -709,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="117">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -918,6 +906,9 @@
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -954,6 +945,9 @@
     <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -978,6 +972,9 @@
     <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -990,12 +987,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="6" applyFont="1" fillId="5" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1038,6 +1029,9 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1045,6 +1039,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1359,19 +1356,19 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="63" width="3.5764285714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="110" width="23.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="111" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="112" width="23.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="113" width="17.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="63" width="6.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="63" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="112" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="114" width="14.719285714285713" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="66" width="6.576428571428571" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="63" width="25.862142857142857" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="63" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="66" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="115" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="63" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="113" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="113" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="113" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="116" width="22.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="116" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="116" width="14.719285714285713" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="63" width="6.576428571428571" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="63" width="21.14785714285714" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="66" width="9.005" customWidth="1" bestFit="1"/>
@@ -1399,9 +1396,9 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="71" t="s">
+      <c r="J1" s="70"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="72" t="s">
         <v>43</v>
       </c>
       <c r="M1" s="3"/>
@@ -1410,1203 +1407,1185 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="21"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="74" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="21"/>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="75" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="69"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="74" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="75" t="s">
         <v>45</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
       <c r="AA2" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="21"/>
-      <c r="B3" s="77">
+      <c r="B3" s="78">
         <v>25568.750295925925</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="79" t="s">
+      <c r="D3" s="71"/>
+      <c r="E3" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="70"/>
-      <c r="H3" s="81" t="s">
+      <c r="G3" s="71"/>
+      <c r="H3" s="82" t="s">
         <v>48</v>
       </c>
       <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="82" t="s">
+      <c r="J3" s="83"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="84" t="s">
         <v>49</v>
       </c>
       <c r="M3" s="40"/>
       <c r="N3" s="40"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="82" t="s">
+      <c r="O3" s="71"/>
+      <c r="P3" s="84" t="s">
         <v>33</v>
       </c>
       <c r="Q3" s="40"/>
       <c r="R3" s="40"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
       <c r="Y3" s="21"/>
       <c r="Z3" s="21"/>
       <c r="AA3" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="21"/>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="70"/>
-      <c r="E4" s="85" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="87" t="s">
+      <c r="G4" s="71"/>
+      <c r="H4" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="88"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="87" t="s">
+      <c r="I4" s="90"/>
+      <c r="J4" s="91">
+        <v>637</v>
+      </c>
+      <c r="K4" s="71"/>
+      <c r="L4" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="88"/>
-      <c r="N4" s="90" t="s">
+      <c r="M4" s="90"/>
+      <c r="N4" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="70"/>
-      <c r="P4" s="87" t="s">
+      <c r="O4" s="71"/>
+      <c r="P4" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="71"/>
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="21"/>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="91">
-        <v>1546.44</v>
-      </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="85" t="s">
+      <c r="C5" s="94">
+        <v>1338.33</v>
+      </c>
+      <c r="D5" s="71"/>
+      <c r="E5" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="87" t="s">
+      <c r="G5" s="71"/>
+      <c r="H5" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="88"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="87" t="s">
+      <c r="I5" s="90"/>
+      <c r="J5" s="95">
+        <v>39.02</v>
+      </c>
+      <c r="K5" s="71"/>
+      <c r="L5" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="M5" s="88"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="87" t="s">
+      <c r="M5" s="90"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
       <c r="Y5" s="21"/>
       <c r="Z5" s="21"/>
       <c r="AA5" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="21"/>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="85" t="s">
+      <c r="C6" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="71"/>
+      <c r="E6" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="90">
+      <c r="F6" s="93">
         <v>16350.88</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="87" t="s">
+      <c r="G6" s="71"/>
+      <c r="H6" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="88"/>
-      <c r="J6" s="94" t="s">
+      <c r="I6" s="90"/>
+      <c r="J6" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="70"/>
-      <c r="L6" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="88"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="87" t="s">
+      <c r="K6" s="71"/>
+      <c r="L6" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="70"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="89" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
+      <c r="X6" s="71"/>
       <c r="Y6" s="21"/>
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="21"/>
-      <c r="B7" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="93">
-        <v>133</v>
-      </c>
-      <c r="D7" s="70"/>
-      <c r="E7" s="85" t="s">
+      <c r="B7" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="96">
+      <c r="C7" s="96">
+        <v>131</v>
+      </c>
+      <c r="D7" s="71"/>
+      <c r="E7" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="97">
         <v>4318.11</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="87" t="s">
+      <c r="G7" s="71"/>
+      <c r="H7" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="90"/>
+      <c r="J7" s="93">
+        <v>215.85</v>
+      </c>
+      <c r="K7" s="71"/>
+      <c r="L7" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="90"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="88"/>
-      <c r="J7" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="70"/>
-      <c r="L7" s="87" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" s="88"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="70"/>
-      <c r="P7" s="87" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="70"/>
-      <c r="T7" s="70"/>
-      <c r="U7" s="70"/>
-      <c r="V7" s="70"/>
-      <c r="W7" s="70"/>
-      <c r="X7" s="70"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="71"/>
+      <c r="X7" s="71"/>
       <c r="Y7" s="21"/>
       <c r="Z7" s="21"/>
       <c r="AA7" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="21"/>
-      <c r="B8" s="97" t="s">
-        <v>69</v>
+      <c r="B8" s="98" t="s">
+        <v>70</v>
       </c>
       <c r="C8" s="62">
-        <v>44.43</v>
-      </c>
-      <c r="D8" s="70"/>
-      <c r="E8" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="86">
+        <v>35.37</v>
+      </c>
+      <c r="D8" s="71"/>
+      <c r="E8" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="88">
         <v>419</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="88"/>
-      <c r="J8" s="90" t="s">
+      <c r="G8" s="71"/>
+      <c r="H8" s="89" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="90"/>
+      <c r="J8" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="70"/>
-      <c r="L8" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="M8" s="88"/>
-      <c r="N8" s="90" t="s">
+      <c r="K8" s="71"/>
+      <c r="L8" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="90"/>
+      <c r="N8" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="O8" s="70"/>
-      <c r="P8" s="87" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="86"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
       <c r="Y8" s="21"/>
       <c r="Z8" s="21"/>
       <c r="AA8" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="21"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="85" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="86" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="90"/>
+      <c r="N9" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="87" t="s">
-        <v>75</v>
-      </c>
-      <c r="M9" s="88"/>
-      <c r="N9" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="O9" s="70"/>
-      <c r="P9" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q9" s="88"/>
-      <c r="R9" s="89"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="91"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="71"/>
+      <c r="X9" s="71"/>
       <c r="Y9" s="21"/>
       <c r="Z9" s="21"/>
       <c r="AA9" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="21"/>
-      <c r="B10" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="75" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="70"/>
-      <c r="H10" s="82" t="s">
+      <c r="B10" s="85" t="s">
         <v>79</v>
       </c>
+      <c r="C10" s="93"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="71"/>
+      <c r="H10" s="84" t="s">
+        <v>81</v>
+      </c>
       <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="M10" s="70"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="70"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="71"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="71"/>
       <c r="P10" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q10" s="99"/>
+        <v>82</v>
+      </c>
+      <c r="Q10" s="100"/>
       <c r="R10" s="61"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
-      <c r="V10" s="70"/>
-      <c r="W10" s="70"/>
-      <c r="X10" s="70"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="71"/>
       <c r="Y10" s="21"/>
       <c r="Z10" s="21"/>
       <c r="AA10" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="21"/>
-      <c r="B11" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="90">
-        <v>5898.57</v>
-      </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="87" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="88"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="82"/>
+      <c r="B11" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="93">
+        <v>4542.67</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="90"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="84"/>
       <c r="M11" s="40"/>
       <c r="N11" s="40"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="101"/>
-      <c r="Q11" s="101"/>
-      <c r="R11" s="101"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="70"/>
-      <c r="U11" s="70"/>
-      <c r="V11" s="70"/>
-      <c r="W11" s="70"/>
-      <c r="X11" s="70"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="102"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="71"/>
       <c r="Y11" s="21"/>
       <c r="Z11" s="21"/>
       <c r="AA11" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="21"/>
-      <c r="B12" s="102" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="103">
-        <v>9.99</v>
-      </c>
-      <c r="D12" s="70"/>
-      <c r="E12" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="96"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="87" t="s">
+      <c r="B12" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="88"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="M12" s="88"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="70"/>
-      <c r="P12" s="85" t="s">
+      <c r="C12" s="104">
+        <v>91.01</v>
+      </c>
+      <c r="D12" s="71"/>
+      <c r="E12" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="97"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="90"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="90"/>
+      <c r="N12" s="97"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="Q12" s="104" t="s">
+      <c r="Q12" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="R12" s="104" t="s">
+      <c r="R12" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="S12" s="70"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="70"/>
-      <c r="V12" s="70"/>
-      <c r="W12" s="70"/>
-      <c r="X12" s="70"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
       <c r="AA12" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="21"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="96" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="70"/>
-      <c r="H13" s="87" t="s">
+      <c r="B13" s="78"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="M13" s="88"/>
-      <c r="N13" s="96"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="85" t="s">
+      <c r="F13" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="70"/>
-      <c r="T13" s="70"/>
-      <c r="U13" s="70"/>
-      <c r="V13" s="70"/>
-      <c r="W13" s="70"/>
-      <c r="X13" s="70"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="90"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="90"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q13" s="105"/>
+      <c r="R13" s="91"/>
+      <c r="S13" s="71"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="71"/>
+      <c r="V13" s="71"/>
+      <c r="W13" s="71"/>
+      <c r="X13" s="71"/>
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
       <c r="AA13" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="21"/>
-      <c r="B14" s="83">
+      <c r="B14" s="85">
         <v>25568.750295925925</v>
       </c>
-      <c r="C14" s="84"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="87" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="87" t="s">
+      <c r="C14" s="86"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="M14" s="88"/>
-      <c r="N14" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="O14" s="70"/>
-      <c r="P14" s="85" t="s">
+      <c r="F14" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="89"/>
-      <c r="S14" s="70"/>
-      <c r="T14" s="70"/>
-      <c r="U14" s="70"/>
-      <c r="V14" s="70"/>
-      <c r="W14" s="70"/>
-      <c r="X14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" s="90"/>
+      <c r="N14" s="105" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" s="71"/>
+      <c r="P14" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q14" s="105"/>
+      <c r="R14" s="91"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="71"/>
+      <c r="V14" s="71"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="71"/>
       <c r="Y14" s="21"/>
       <c r="Z14" s="21"/>
       <c r="AA14" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="21"/>
-      <c r="B15" s="83" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="84">
+      <c r="B15" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="86">
         <v>182</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="87" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="M15" s="70"/>
-      <c r="N15" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="85" t="s">
+      <c r="D15" s="71"/>
+      <c r="E15" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="70"/>
-      <c r="V15" s="70"/>
-      <c r="W15" s="70"/>
-      <c r="X15" s="70"/>
+      <c r="F15" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="71"/>
+      <c r="N15" s="105" t="s">
+        <v>93</v>
+      </c>
+      <c r="O15" s="71"/>
+      <c r="P15" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q15" s="105"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="71"/>
+      <c r="V15" s="71"/>
+      <c r="W15" s="71"/>
+      <c r="X15" s="71"/>
       <c r="Y15" s="21"/>
       <c r="Z15" s="21"/>
       <c r="AA15" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="21"/>
-      <c r="B16" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="84">
+      <c r="B16" s="85" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="86">
         <v>36</v>
       </c>
-      <c r="D16" s="70"/>
-      <c r="E16" s="87" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="82"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="84"/>
       <c r="M16" s="40"/>
       <c r="N16" s="40"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="85" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="89"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="70"/>
-      <c r="U16" s="70"/>
-      <c r="V16" s="70"/>
-      <c r="W16" s="70"/>
-      <c r="X16" s="70"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="91"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="71"/>
+      <c r="V16" s="71"/>
+      <c r="W16" s="71"/>
+      <c r="X16" s="71"/>
       <c r="Y16" s="21"/>
       <c r="Z16" s="21"/>
       <c r="AA16" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="70"/>
-      <c r="B17" s="102" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="103">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="71"/>
+      <c r="B17" s="103" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="104">
         <v>227</v>
       </c>
-      <c r="D17" s="70"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="M17" s="88"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="70"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="70"/>
-      <c r="V17" s="70"/>
-      <c r="W17" s="70"/>
-      <c r="X17" s="70"/>
+        <v>104</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="90"/>
+      <c r="N17" s="97"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="77"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="71"/>
+      <c r="X17" s="71"/>
       <c r="Y17" s="21"/>
       <c r="Z17" s="21"/>
       <c r="AA17" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="70"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="87" t="s">
-        <v>82</v>
-      </c>
-      <c r="M18" s="88"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="70"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="76"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="70"/>
-      <c r="V18" s="70"/>
-      <c r="W18" s="70"/>
-      <c r="X18" s="70"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18" s="90"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="71"/>
+      <c r="R18" s="77"/>
+      <c r="S18" s="71"/>
+      <c r="T18" s="71"/>
+      <c r="U18" s="71"/>
+      <c r="V18" s="71"/>
+      <c r="W18" s="71"/>
+      <c r="X18" s="71"/>
       <c r="Y18" s="21"/>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="70"/>
-      <c r="B19" s="83">
+      <c r="A19" s="71"/>
+      <c r="B19" s="85">
         <v>25568.750295925925</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="87" t="s">
-        <v>85</v>
-      </c>
-      <c r="M19" s="88"/>
-      <c r="N19" s="96"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="76"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
-      <c r="W19" s="70"/>
-      <c r="X19" s="70"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="M19" s="90"/>
+      <c r="N19" s="97"/>
+      <c r="O19" s="71"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
+      <c r="R19" s="77"/>
+      <c r="S19" s="71"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="71"/>
+      <c r="X19" s="71"/>
       <c r="Y19" s="21"/>
       <c r="Z19" s="21"/>
       <c r="AA19" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="70"/>
-      <c r="B20" s="83" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="93">
+      <c r="A20" s="71"/>
+      <c r="B20" s="85" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="96">
         <v>814</v>
       </c>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="70"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="M20" s="70"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="70"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="70"/>
-      <c r="U20" s="70"/>
-      <c r="V20" s="70"/>
-      <c r="W20" s="70"/>
-      <c r="X20" s="70"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="71"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="71"/>
+      <c r="R20" s="77"/>
+      <c r="S20" s="71"/>
+      <c r="T20" s="71"/>
+      <c r="U20" s="71"/>
+      <c r="V20" s="71"/>
+      <c r="W20" s="71"/>
+      <c r="X20" s="71"/>
       <c r="Y20" s="21"/>
       <c r="Z20" s="21"/>
       <c r="AA20" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="70"/>
-      <c r="B21" s="102" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="103">
+      <c r="A21" s="71"/>
+      <c r="B21" s="103" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="104">
         <v>22</v>
       </c>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="70"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="70"/>
-      <c r="X21" s="70"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="77"/>
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="71"/>
+      <c r="V21" s="71"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="71"/>
       <c r="Y21" s="21"/>
       <c r="Z21" s="21"/>
       <c r="AA21" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="70"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="70"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="76"/>
-      <c r="S22" s="70"/>
-      <c r="T22" s="70"/>
-      <c r="U22" s="70"/>
-      <c r="V22" s="70"/>
-      <c r="W22" s="70"/>
-      <c r="X22" s="70"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="71"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="77"/>
+      <c r="S22" s="71"/>
+      <c r="T22" s="71"/>
+      <c r="U22" s="71"/>
+      <c r="V22" s="71"/>
+      <c r="W22" s="71"/>
+      <c r="X22" s="71"/>
       <c r="Y22" s="21"/>
       <c r="Z22" s="21"/>
       <c r="AA22" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="70"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="70"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="70"/>
-      <c r="L23" s="70"/>
-      <c r="M23" s="70"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="70"/>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="70"/>
-      <c r="R23" s="76"/>
-      <c r="S23" s="70"/>
-      <c r="T23" s="70"/>
-      <c r="U23" s="70"/>
-      <c r="V23" s="70"/>
-      <c r="W23" s="70"/>
-      <c r="X23" s="70"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="71"/>
+      <c r="R23" s="77"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="71"/>
+      <c r="V23" s="71"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="71"/>
       <c r="Y23" s="21"/>
       <c r="Z23" s="21"/>
       <c r="AA23" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="70"/>
-      <c r="B24" s="102"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="70"/>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="70"/>
-      <c r="R24" s="76"/>
-      <c r="S24" s="70"/>
-      <c r="T24" s="70"/>
-      <c r="U24" s="70"/>
-      <c r="V24" s="70"/>
-      <c r="W24" s="70"/>
-      <c r="X24" s="70"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="76"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="77"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="71"/>
+      <c r="U24" s="71"/>
+      <c r="V24" s="71"/>
+      <c r="W24" s="71"/>
+      <c r="X24" s="71"/>
       <c r="Y24" s="21"/>
       <c r="Z24" s="21"/>
       <c r="AA24" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="70"/>
-      <c r="B25" s="102"/>
-      <c r="C25" s="103"/>
-      <c r="D25" s="70"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="70"/>
-      <c r="M25" s="70"/>
-      <c r="N25" s="75"/>
-      <c r="O25" s="70"/>
-      <c r="P25" s="70"/>
-      <c r="Q25" s="70"/>
-      <c r="R25" s="76"/>
-      <c r="S25" s="70"/>
-      <c r="T25" s="70"/>
-      <c r="U25" s="70"/>
-      <c r="V25" s="70"/>
-      <c r="W25" s="70"/>
-      <c r="X25" s="70"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="76"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="77"/>
+      <c r="S25" s="71"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="71"/>
+      <c r="V25" s="71"/>
+      <c r="W25" s="71"/>
+      <c r="X25" s="71"/>
       <c r="Y25" s="21"/>
       <c r="Z25" s="21"/>
       <c r="AA25" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="21"/>
-      <c r="B26" s="97"/>
+      <c r="B26" s="98"/>
       <c r="C26" s="62"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="81"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="81"/>
+      <c r="J26" s="83"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="82"/>
       <c r="Q26" s="40"/>
       <c r="R26" s="40"/>
-      <c r="S26" s="70"/>
-      <c r="T26" s="70"/>
-      <c r="U26" s="70"/>
-      <c r="V26" s="70"/>
-      <c r="W26" s="70"/>
-      <c r="X26" s="70"/>
+      <c r="S26" s="71"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="71"/>
+      <c r="V26" s="71"/>
+      <c r="W26" s="71"/>
+      <c r="X26" s="71"/>
       <c r="Y26" s="21"/>
       <c r="Z26" s="21"/>
       <c r="AA26" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="21"/>
-      <c r="B27" s="97"/>
+      <c r="B27" s="98"/>
       <c r="C27" s="62"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" s="105"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="75"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="87"/>
-      <c r="Q27" s="88"/>
-      <c r="R27" s="90"/>
-      <c r="S27" s="70"/>
-      <c r="T27" s="70"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="70"/>
-      <c r="W27" s="70"/>
-      <c r="X27" s="70"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="71"/>
+      <c r="N27" s="76"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="90"/>
+      <c r="R27" s="93"/>
+      <c r="S27" s="71"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="71"/>
+      <c r="V27" s="71"/>
+      <c r="W27" s="71"/>
+      <c r="X27" s="71"/>
       <c r="Y27" s="21"/>
       <c r="Z27" s="21"/>
       <c r="AA27" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="21"/>
-      <c r="B28" s="97"/>
+      <c r="B28" s="98"/>
       <c r="C28" s="62"/>
       <c r="D28" s="21"/>
-      <c r="E28" s="106" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" s="107"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="70"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="75"/>
-      <c r="O28" s="70"/>
-      <c r="P28" s="87" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q28" s="88"/>
-      <c r="R28" s="90"/>
-      <c r="S28" s="70"/>
-      <c r="T28" s="70"/>
-      <c r="U28" s="70"/>
-      <c r="V28" s="70"/>
-      <c r="W28" s="70"/>
-      <c r="X28" s="70"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="90"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="71"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="71"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="71"/>
+      <c r="X28" s="71"/>
       <c r="Y28" s="21"/>
       <c r="Z28" s="21"/>
       <c r="AA28" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="21"/>
-      <c r="B29" s="97"/>
+      <c r="B29" s="98"/>
       <c r="C29" s="62"/>
       <c r="D29" s="21"/>
-      <c r="E29" s="106" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="107"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="88"/>
-      <c r="J29" s="90"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="93"/>
       <c r="K29" s="21"/>
-      <c r="L29" s="70"/>
-      <c r="M29" s="70"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="70"/>
-      <c r="P29" s="87" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q29" s="88"/>
-      <c r="R29" s="90"/>
-      <c r="S29" s="70"/>
-      <c r="T29" s="70"/>
-      <c r="U29" s="70"/>
-      <c r="V29" s="70"/>
-      <c r="W29" s="70"/>
-      <c r="X29" s="70"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="71"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="93"/>
+      <c r="S29" s="71"/>
+      <c r="T29" s="71"/>
+      <c r="U29" s="71"/>
+      <c r="V29" s="71"/>
+      <c r="W29" s="71"/>
+      <c r="X29" s="71"/>
       <c r="Y29" s="21"/>
       <c r="Z29" s="21"/>
       <c r="AA29" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="21"/>
-      <c r="B30" s="97"/>
+      <c r="B30" s="98"/>
       <c r="C30" s="62"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" s="105"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="88"/>
-      <c r="J30" s="90"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="93"/>
       <c r="K30" s="21"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="70"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="70"/>
-      <c r="P30" s="87" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q30" s="88"/>
-      <c r="R30" s="90"/>
-      <c r="S30" s="70"/>
-      <c r="T30" s="70"/>
-      <c r="U30" s="70"/>
-      <c r="V30" s="70"/>
-      <c r="W30" s="70"/>
-      <c r="X30" s="70"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="76"/>
+      <c r="O30" s="71"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="90"/>
+      <c r="R30" s="93"/>
+      <c r="S30" s="71"/>
+      <c r="T30" s="71"/>
+      <c r="U30" s="71"/>
+      <c r="V30" s="71"/>
+      <c r="W30" s="71"/>
+      <c r="X30" s="71"/>
       <c r="Y30" s="21"/>
       <c r="Z30" s="21"/>
       <c r="AA30" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="21"/>
-      <c r="B31" s="97"/>
+      <c r="B31" s="98"/>
       <c r="C31" s="62"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" s="105"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="88"/>
-      <c r="J31" s="89"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="90"/>
+      <c r="J31" s="91"/>
       <c r="K31" s="21"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="75"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="87" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q31" s="88"/>
-      <c r="R31" s="108"/>
-      <c r="S31" s="70"/>
-      <c r="T31" s="70"/>
-      <c r="U31" s="70"/>
-      <c r="V31" s="70"/>
-      <c r="W31" s="70"/>
-      <c r="X31" s="70"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+      <c r="N31" s="76"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="89"/>
+      <c r="Q31" s="90"/>
+      <c r="R31" s="109"/>
+      <c r="S31" s="71"/>
+      <c r="T31" s="71"/>
+      <c r="U31" s="71"/>
+      <c r="V31" s="71"/>
+      <c r="W31" s="71"/>
+      <c r="X31" s="71"/>
       <c r="Y31" s="21"/>
       <c r="Z31" s="21"/>
       <c r="AA31" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="21"/>
-      <c r="B32" s="97"/>
+      <c r="B32" s="98"/>
       <c r="C32" s="62"/>
       <c r="D32" s="21"/>
-      <c r="E32" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" s="105"/>
-      <c r="G32" s="99"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="100"/>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
       <c r="J32" s="61"/>
       <c r="K32" s="21"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="70"/>
-      <c r="P32" s="70" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q32" s="70"/>
-      <c r="R32" s="76"/>
-      <c r="S32" s="70"/>
-      <c r="T32" s="70"/>
-      <c r="U32" s="70"/>
-      <c r="V32" s="70"/>
-      <c r="W32" s="70"/>
-      <c r="X32" s="70"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="76"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+      <c r="R32" s="77"/>
+      <c r="S32" s="71"/>
+      <c r="T32" s="71"/>
+      <c r="U32" s="71"/>
+      <c r="V32" s="71"/>
+      <c r="W32" s="71"/>
+      <c r="X32" s="71"/>
       <c r="Y32" s="21"/>
       <c r="Z32" s="21"/>
       <c r="AA32" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="21"/>
-      <c r="B33" s="97"/>
+      <c r="B33" s="98"/>
       <c r="C33" s="62"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="99"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="100"/>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
       <c r="J33" s="61"/>
       <c r="K33" s="21"/>
-      <c r="L33" s="109"/>
-      <c r="M33" s="109"/>
-      <c r="N33" s="105"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="110"/>
+      <c r="N33" s="106"/>
       <c r="O33" s="21"/>
-      <c r="P33" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q33" s="99"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="100"/>
       <c r="R33" s="61"/>
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
-      <c r="W33" s="70"/>
-      <c r="X33" s="70"/>
+      <c r="W33" s="71"/>
+      <c r="X33" s="71"/>
       <c r="Y33" s="21"/>
       <c r="Z33" s="21"/>
       <c r="AA33" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="21"/>
-      <c r="B34" s="97"/>
+      <c r="B34" s="98"/>
       <c r="C34" s="61"/>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="105"/>
-      <c r="G34" s="99"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="100"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
-      <c r="J34" s="99"/>
+      <c r="J34" s="111"/>
       <c r="K34" s="21"/>
-      <c r="L34" s="109"/>
-      <c r="M34" s="109"/>
-      <c r="N34" s="109"/>
+      <c r="L34" s="110"/>
+      <c r="M34" s="110"/>
+      <c r="N34" s="110"/>
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
-      <c r="Q34" s="99"/>
-      <c r="R34" s="99"/>
+      <c r="Q34" s="100"/>
+      <c r="R34" s="100"/>
       <c r="S34" s="21"/>
       <c r="T34" s="21"/>
       <c r="U34" s="21"/>

</xml_diff>